<commit_message>
final changes without json password
</commit_message>
<xml_diff>
--- a/spat_dashboard/company_summary.xlsx
+++ b/spat_dashboard/company_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'Customer Service': 4, 'Communication': 1, 'Ease of Process': 2, 'Safety and Care': 4, 'Reputation': 4}</t>
+          <t>{'Customer Service': 4, 'Communication': 1, 'Ease of Process': 3, 'Safety and Care': 5, 'Reputation': 4}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'Customer Service': 5, 'Communication': 2, 'Ease of Process': 2, 'Safety and Care': 2, 'Reputation': 3}</t>
+          <t>{'Customer Service': 3, 'Safety and Care': 1, 'Reputation': 2}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'Customer Service': 16, 'Pricing': 4, 'Communication': 5, 'Ease of Process': 11, 'Safety and Care': 10, 'Reputation': 17}</t>
+          <t>{'Customer Service': 18, 'Pricing': 4, 'Communication': 6, 'Ease of Process': 12, 'Safety and Care': 11, 'Reputation': 19}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{'Customer Service': 7, 'Pricing': 2, 'Communication': 3, 'Ease of Process': 10, 'Safety and Care': 8, 'Reputation': 13}</t>
+          <t>{'Customer Service': 9, 'Pricing': 2, 'Communication': 4, 'Ease of Process': 12, 'Safety and Care': 9, 'Reputation': 13}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'Customer Service': 6, 'Pricing': 2, 'Communication': 3, 'Ease of Process': 3, 'Safety and Care': 2, 'Reputation': 6}</t>
+          <t>{'Customer Service': 3, 'Communication': 2, 'Ease of Process': 1, 'Safety and Care': 1, 'Reputation': 4}</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{'Customer Service': 7, 'Communication': 2, 'Ease of Process': 5, 'Safety and Care': 5, 'Reputation': 6}</t>
+          <t>{'Customer Service': 6, 'Communication': 2, 'Ease of Process': 6, 'Safety and Care': 4, 'Reputation': 5}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'Customer Service': 119, 'Pricing': 16, 'Communication': 51, 'Ease of Process': 96, 'Safety and Care': 93, 'Reputation': 106}</t>
+          <t>{'Customer Service': 113, 'Pricing': 15, 'Communication': 48, 'Ease of Process': 92, 'Safety and Care': 87, 'Reputation': 102}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'Customer Service': 3, 'Pricing': 4, 'Communication': 2, 'Ease of Process': 2, 'Safety and Care': 3, 'Reputation': 4}</t>
+          <t>{'Customer Service': 2, 'Communication': 2, 'Ease of Process': 1, 'Safety and Care': 2, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{'Customer Service': 112, 'Pricing': 19, 'Communication': 32, 'Ease of Process': 89, 'Safety and Care': 90, 'Reputation': 98}</t>
+          <t>{'Customer Service': 111, 'Pricing': 17, 'Communication': 30, 'Ease of Process': 85, 'Safety and Care': 85, 'Reputation': 96}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'Customer Service': 2, 'Ease of Process': 1, 'Reputation': 2}</t>
+          <t>{'Customer Service': 1, 'Ease of Process': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Safety and Care': 4, 'Reputation': 2}</t>
+          <t>{'Customer Service': 1, 'Safety and Care': 2, 'Reputation': 1}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'Ease of Process': 1, 'Reputation': 2}</t>
+          <t>{'Ease of Process': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{'Customer Service': 63, 'Pricing': 4, 'Communication': 22, 'Ease of Process': 59, 'Safety and Care': 52, 'Reputation': 67}</t>
+          <t>{'Customer Service': 64, 'Pricing': 4, 'Communication': 22, 'Ease of Process': 59, 'Safety and Care': 52, 'Reputation': 67}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'Customer Service': 5, 'Communication': 2, 'Ease of Process': 2, 'Safety and Care': 3, 'Reputation': 3}</t>
+          <t>{'Customer Service': 3, 'Communication': 2, 'Ease of Process': 2, 'Safety and Care': 1, 'Reputation': 2}</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{'Customer Service': 11, 'Pricing': 2, 'Communication': 4, 'Ease of Process': 9, 'Safety and Care': 9, 'Reputation': 10}</t>
+          <t>{'Customer Service': 11, 'Pricing': 2, 'Communication': 3, 'Ease of Process': 8, 'Safety and Care': 9, 'Reputation': 9}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'Safety and Care': 1, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{'Customer Service': 34, 'Pricing': 1, 'Communication': 4, 'Ease of Process': 30, 'Safety and Care': 13, 'Reputation': 39}</t>
+          <t>{'Customer Service': 36, 'Pricing': 1, 'Communication': 5, 'Ease of Process': 32, 'Safety and Care': 13, 'Reputation': 40}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'Customer Service': 2, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{'Customer Service': 27, 'Pricing': 3, 'Communication': 6, 'Ease of Process': 25, 'Safety and Care': 21, 'Reputation': 32}</t>
+          <t>{'Customer Service': 23, 'Pricing': 2, 'Communication': 5, 'Ease of Process': 21, 'Safety and Care': 19, 'Reputation': 31}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'Pricing': 1, 'Communication': 1, 'Ease of Process': 1, 'Safety and Care': 1, 'Reputation': 2}</t>
+          <t>{'Reputation': 1}</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{'Customer Service': 88, 'Pricing': 6, 'Communication': 40, 'Ease of Process': 83, 'Safety and Care': 68, 'Reputation': 101}</t>
+          <t>{'Customer Service': 88, 'Pricing': 6, 'Communication': 42, 'Ease of Process': 83, 'Safety and Care': 68, 'Reputation': 96}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{'Customer Service': 11, 'Pricing': 1, 'Communication': 5, 'Ease of Process': 7, 'Safety and Care': 5, 'Reputation': 9}</t>
+          <t>{'Customer Service': 10, 'Communication': 4, 'Ease of Process': 6, 'Safety and Care': 4, 'Reputation': 8}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'Communication': 1, 'Safety and Care': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{'Customer Service': 12, 'Communication': 2, 'Ease of Process': 6, 'Safety and Care': 13, 'Reputation': 13}</t>
+          <t>{'Customer Service': 12, 'Communication': 2, 'Ease of Process': 7, 'Safety and Care': 13, 'Reputation': 13}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>{'Customer Service': 62, 'Pricing': 10, 'Communication': 18, 'Ease of Process': 58, 'Safety and Care': 44, 'Reputation': 58}</t>
+          <t>{'Customer Service': 63, 'Pricing': 9, 'Communication': 16, 'Ease of Process': 56, 'Safety and Care': 43, 'Reputation': 58}</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{'Customer Service': 78, 'Pricing': 8, 'Communication': 53, 'Ease of Process': 68, 'Safety and Care': 76, 'Reputation': 82}</t>
+          <t>{'Customer Service': 82, 'Pricing': 8, 'Communication': 53, 'Ease of Process': 68, 'Safety and Care': 79, 'Reputation': 85}</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Communication': 2, 'Reputation': 2}</t>
+          <t>{'Reputation': 1}</t>
         </is>
       </c>
     </row>
@@ -849,12 +849,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{'Customer Service': 95, 'Pricing': 16, 'Communication': 51, 'Ease of Process': 107, 'Safety and Care': 85, 'Reputation': 105}</t>
+          <t>{'Customer Service': 95, 'Pricing': 16, 'Communication': 51, 'Ease of Process': 107, 'Safety and Care': 87, 'Reputation': 104}</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'Customer Service': 2, 'Ease of Process': 1, 'Reputation': 1}</t>
+          <t>{'Customer Service': 1}</t>
         </is>
       </c>
     </row>
@@ -866,245 +866,245 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{'Customer Service': 6, 'Pricing': 3, 'Ease of Process': 4, 'Safety and Care': 6, 'Reputation': 4}</t>
+          <t>{'Customer Service': 6, 'Pricing': 2, 'Ease of Process': 4, 'Safety and Care': 6, 'Reputation': 3}</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Pricing': 1, 'Communication': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lisa Meador Schoppa- Animal Travel Agent</t>
+          <t>Merflex International Inc</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
+          <t>{'Customer Service': 44, 'Pricing': 3, 'Communication': 3, 'Ease of Process': 4, 'Safety and Care': 18, 'Reputation': 34}</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'Customer Service': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Merflex International Inc</t>
+          <t>Move Pets</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>{'Customer Service': 44, 'Pricing': 3, 'Communication': 3, 'Ease of Process': 4, 'Safety and Care': 18, 'Reputation': 34}</t>
+          <t>{'Customer Service': 5, 'Communication': 1, 'Ease of Process': 5, 'Safety and Care': 3, 'Reputation': 3}</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Move Pets</t>
+          <t>The ARK at JFK</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>{'Customer Service': 4, 'Communication': 1, 'Ease of Process': 4, 'Safety and Care': 3, 'Reputation': 3}</t>
+          <t>{'Customer Service': 45, 'Pricing': 2, 'Communication': 7, 'Ease of Process': 18, 'Safety and Care': 20, 'Reputation': 30}</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'Customer Service': 4, 'Pricing': 1, 'Ease of Process': 1, 'Safety and Care': 4, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>The ARK at JFK</t>
+          <t>Pack Your Pets Pet Travel</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>{'Customer Service': 47, 'Pricing': 3, 'Communication': 7, 'Ease of Process': 20, 'Safety and Care': 22, 'Reputation': 29}</t>
+          <t>{'Customer Service': 8, 'Pricing': 3, 'Communication': 1, 'Ease of Process': 9, 'Safety and Care': 7, 'Reputation': 9}</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'Customer Service': 10, 'Pricing': 4, 'Ease of Process': 3, 'Safety and Care': 7, 'Reputation': 4}</t>
+          <t>{'Pricing': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Pack Your Pets Pet Travel</t>
+          <t>Peace of Mind Pet Shipping &amp; Resort</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>{'Customer Service': 9, 'Pricing': 3, 'Communication': 1, 'Ease of Process': 9, 'Safety and Care': 7, 'Reputation': 10}</t>
+          <t>{'Customer Service': 14, 'Pricing': 2, 'Communication': 4, 'Ease of Process': 11, 'Safety and Care': 13, 'Reputation': 18}</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'Pricing': 1, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Peace of Mind Pet Shipping &amp; Resort</t>
+          <t>Pender AIR</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>{'Customer Service': 13, 'Pricing': 2, 'Communication': 4, 'Ease of Process': 11, 'Safety and Care': 12, 'Reputation': 17}</t>
+          <t>{'Customer Service': 108, 'Pricing': 23, 'Communication': 28, 'Ease of Process': 83, 'Safety and Care': 77, 'Reputation': 94}</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'Customer Service': 1, 'Pricing': 1, 'Ease of Process': 1, 'Reputation': 2}</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Pender AIR</t>
+          <t>Pet Air Carrier</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>{'Customer Service': 106, 'Pricing': 23, 'Communication': 28, 'Ease of Process': 86, 'Safety and Care': 76, 'Reputation': 94}</t>
+          <t>{'Customer Service': 35, 'Pricing': 3, 'Communication': 8, 'Ease of Process': 28, 'Safety and Care': 23, 'Reputation': 26}</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'Customer Service': 2, 'Pricing': 2, 'Communication': 1, 'Ease of Process': 2, 'Safety and Care': 1, 'Reputation': 3}</t>
+          <t>{'Customer Service': 2, 'Ease of Process': 1}</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Pet Air Carrier</t>
+          <t>Pet Cargo, LLC</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>{'Customer Service': 36, 'Pricing': 3, 'Communication': 8, 'Ease of Process': 27, 'Safety and Care': 23, 'Reputation': 26}</t>
+          <t>{'Customer Service': 10, 'Communication': 4, 'Ease of Process': 3, 'Safety and Care': 9, 'Reputation': 15}</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'Customer Service': 3, 'Pricing': 1, 'Ease of Process': 1, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Pet Cargo, LLC</t>
+          <t>Pet Chauffeur</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>{'Customer Service': 9, 'Communication': 4, 'Ease of Process': 3, 'Safety and Care': 7, 'Reputation': 15}</t>
+          <t>{'Customer Service': 50, 'Pricing': 5, 'Communication': 10, 'Ease of Process': 23, 'Safety and Care': 32, 'Reputation': 49}</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1}</t>
+          <t>{'Customer Service': 3, 'Pricing': 1, 'Ease of Process': 1, 'Safety and Care': 2, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Pet Chauffeur</t>
+          <t>Pet Limo Animal Services, Inc</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>{'Customer Service': 52, 'Pricing': 5, 'Communication': 10, 'Ease of Process': 23, 'Safety and Care': 33, 'Reputation': 50}</t>
+          <t>{'Customer Service': 67, 'Pricing': 3, 'Communication': 10, 'Ease of Process': 26, 'Safety and Care': 56, 'Reputation': 37}</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'Customer Service': 3, 'Pricing': 1, 'Ease of Process': 1, 'Safety and Care': 2, 'Reputation': 1}</t>
+          <t>{'Customer Service': 2, 'Pricing': 1, 'Ease of Process': 2, 'Safety and Care': 3}</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Pet Limo Animal Services, Inc</t>
+          <t>Pet Pros Services</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>{'Customer Service': 38, 'Pricing': 5, 'Communication': 10, 'Ease of Process': 23, 'Safety and Care': 47, 'Reputation': 32}</t>
+          <t>{'Customer Service': 31, 'Pricing': 1, 'Communication': 7, 'Ease of Process': 13, 'Safety and Care': 20, 'Reputation': 19}</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'Customer Service': 25, 'Pricing': 5, 'Communication': 8, 'Ease of Process': 5, 'Safety and Care': 16, 'Reputation': 12}</t>
+          <t>{'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Pet Pros Services</t>
+          <t>Pet Relocator</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>{'Customer Service': 30, 'Pricing': 3, 'Communication': 6, 'Ease of Process': 12, 'Safety and Care': 18, 'Reputation': 19}</t>
+          <t>{'Customer Service': 42, 'Pricing': 16, 'Communication': 20, 'Ease of Process': 48, 'Safety and Care': 31, 'Reputation': 48}</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'Reputation': 1}</t>
+          <t>{'Customer Service': 1, 'Ease of Process': 1, 'Safety and Care': 2}</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Pet Relocator</t>
+          <t>Pet Transport PRO</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>{'Customer Service': 42, 'Pricing': 16, 'Communication': 20, 'Ease of Process': 47, 'Safety and Care': 31, 'Reputation': 47}</t>
+          <t>{'Customer Service': 21, 'Pricing': 4, 'Communication': 2, 'Ease of Process': 14, 'Safety and Care': 16, 'Reputation': 29}</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Ease of Process': 1, 'Safety and Care': 2}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Pet Transport PRO</t>
+          <t>Pet Travel Transport</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>{'Customer Service': 21, 'Pricing': 5, 'Communication': 2, 'Ease of Process': 14, 'Safety and Care': 16, 'Reputation': 29}</t>
+          <t>{'Customer Service': 83, 'Pricing': 11, 'Communication': 52, 'Ease of Process': 51, 'Safety and Care': 83, 'Reputation': 85}</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1116,114 +1116,114 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Pet Travel Transport</t>
+          <t>Pet Relocation</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>{'Customer Service': 85, 'Pricing': 12, 'Communication': 55, 'Ease of Process': 50, 'Safety and Care': 85, 'Reputation': 84}</t>
+          <t>{'Customer Service': 86, 'Pricing': 13, 'Communication': 31, 'Ease of Process': 68, 'Safety and Care': 61, 'Reputation': 68}</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pet Relocation</t>
+          <t>Pets in Transit</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>{'Customer Service': 87, 'Pricing': 15, 'Communication': 33, 'Ease of Process': 68, 'Safety and Care': 62, 'Reputation': 70}</t>
+          <t>{'Customer Service': 18, 'Pricing': 1, 'Communication': 3, 'Ease of Process': 12, 'Safety and Care': 12, 'Reputation': 18}</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Pricing': 2, 'Communication': 2, 'Safety and Care': 2, 'Reputation': 2}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Pets in Transit</t>
+          <t>Pets 4 Jets LLC</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{'Customer Service': 15, 'Pricing': 1, 'Communication': 2, 'Ease of Process': 9, 'Safety and Care': 8, 'Reputation': 15}</t>
+          <t>{'Customer Service': 24, 'Pricing': 1, 'Communication': 5, 'Ease of Process': 17, 'Safety and Care': 17, 'Reputation': 25}</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'Communication': 1}</t>
+          <t>{'Customer Service': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Pets 4 Jets LLC</t>
+          <t>Petsfly.Com</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{'Customer Service': 25, 'Pricing': 2, 'Communication': 6, 'Ease of Process': 17, 'Safety and Care': 18, 'Reputation': 26}</t>
+          <t>{'Customer Service': 52, 'Pricing': 9, 'Communication': 25, 'Ease of Process': 50, 'Safety and Care': 42, 'Reputation': 61}</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'Customer Service': 3, 'Pricing': 1, 'Communication': 1, 'Ease of Process': 1, 'Reputation': 3}</t>
+          <t>{'Customer Service': 1, 'Pricing': 1, 'Communication': 1, 'Ease of Process': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Petsfly.Com</t>
+          <t>PETWORK TRAVEL</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{'Customer Service': 50, 'Pricing': 9, 'Communication': 25, 'Ease of Process': 49, 'Safety and Care': 43, 'Reputation': 57}</t>
+          <t>{'Customer Service': 84, 'Pricing': 3, 'Communication': 34, 'Ease of Process': 86, 'Safety and Care': 94, 'Reputation': 81}</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Pricing': 1, 'Communication': 1, 'Ease of Process': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
+          <t>{'Customer Service': 1, 'Communication': 1, 'Ease of Process': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>PETWORK TRAVEL</t>
+          <t>Police Service Dogs, Inc.</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{'Customer Service': 84, 'Pricing': 3, 'Communication': 34, 'Ease of Process': 87, 'Safety and Care': 94, 'Reputation': 83}</t>
+          <t>{}</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'Customer Service': 1, 'Communication': 2, 'Ease of Process': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
+          <t>{}</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Police Service Dogs, Inc.</t>
+          <t>Precious Pets Transport Service, LLC</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'Customer Service': 8, 'Communication': 5, 'Ease of Process': 2, 'Safety and Care': 5, 'Reputation': 7}</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1235,34 +1235,238 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Precious Pets Transport Service, LLC</t>
+          <t>Professional Pet Transport</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{'Customer Service': 8, 'Communication': 5, 'Ease of Process': 2, 'Safety and Care': 5, 'Reputation': 7}</t>
+          <t>{'Customer Service': 11, 'Pricing': 1, 'Communication': 3, 'Ease of Process': 7, 'Safety and Care': 14, 'Reputation': 18}</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'Reputation': 1}</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Professional Pet Transport</t>
+          <t>ShipMyPets.com</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{'Customer Service': 10, 'Pricing': 1, 'Communication': 3, 'Ease of Process': 6, 'Safety and Care': 13, 'Reputation': 16}</t>
+          <t>{'Customer Service': 11, 'Communication': 3, 'Ease of Process': 12, 'Safety and Care': 12, 'Reputation': 12}</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SMART Pet Air Travel</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 87, 'Pricing': 17, 'Communication': 36, 'Ease of Process': 64, 'Safety and Care': 57, 'Reputation': 83}</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 2, 'Ease of Process': 2, 'Reputation': 2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Southern California Pet Transport</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 14, 'Pricing': 2, 'Communication': 2, 'Ease of Process': 15, 'Safety and Care': 16, 'Reputation': 15}</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Starwood Pet Travel</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 96, 'Pricing': 16, 'Communication': 39, 'Ease of Process': 87, 'Safety and Care': 75, 'Reputation': 80}</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 1, 'Pricing': 1, 'Ease of Process': 1, 'Reputation': 2}</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>swissridge kennels</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 6, 'Ease of Process': 3, 'Safety and Care': 5, 'Reputation': 10}</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Tails In The Air</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 1, 'Safety and Care': 2, 'Reputation': 1}</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Tails of Hawaii</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 50, 'Pricing': 2, 'Communication': 13, 'Ease of Process': 12, 'Safety and Care': 76, 'Reputation': 42}</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 3, 'Pricing': 2, 'Ease of Process': 1, 'Safety and Care': 2, 'Reputation': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Tailwind Global Pet</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 58, 'Pricing': 7, 'Communication': 22, 'Ease of Process': 61, 'Safety and Care': 47, 'Reputation': 53}</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 2, 'Pricing': 1, 'Safety and Care': 1, 'Reputation': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Luxe Pet Resort</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 10, 'Pricing': 1, 'Communication': 3, 'Safety and Care': 21, 'Reputation': 5}</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 2, 'Safety and Care': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>The Pet Porters - Pet Transportation Services</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 45, 'Pricing': 3, 'Communication': 26, 'Ease of Process': 36, 'Safety and Care': 51, 'Reputation': 60}</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>{'Reputation': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Transcontinental Pet Movers LLC</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 28, 'Pricing': 6, 'Communication': 7, 'Ease of Process': 25, 'Safety and Care': 27, 'Reputation': 39}</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 1, 'Pricing': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>World Pet Travel</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 56, 'Pricing': 10, 'Communication': 11, 'Ease of Process': 32, 'Safety and Care': 44, 'Reputation': 45}</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 2, 'Communication': 1, 'Ease of Process': 1, 'Reputation': 1}</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>WorldCare Pet Transport</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 122, 'Pricing': 6, 'Communication': 41, 'Ease of Process': 68, 'Safety and Care': 128, 'Reputation': 77}</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>{'Customer Service': 1, 'Ease of Process': 1, 'Safety and Care': 1}</t>
         </is>
       </c>
     </row>

</xml_diff>